<commit_message>
pattern/color fill a cell
</commit_message>
<xml_diff>
--- a/Openpyxl/Example.xlsx
+++ b/Openpyxl/Example.xlsx
@@ -46,12 +46,17 @@
       <sz val="12"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00B60C50"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -66,13 +71,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,7 +528,7 @@
           <t>Tim</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" s="4" t="n">
         <v>1400</v>
       </c>
       <c r="C5" s="3" t="n">

</xml_diff>

<commit_message>
set cell B7 borders
</commit_message>
<xml_diff>
--- a/Openpyxl/Example.xlsx
+++ b/Openpyxl/Example.xlsx
@@ -35,14 +35,14 @@
     </font>
     <font>
       <name val="Arial Black"/>
-      <color rgb="001807FF"/>
+      <color rgb="FF1807FF"/>
       <sz val="14"/>
     </font>
     <font>
       <name val="Arial Black"/>
       <b val="1"/>
       <i val="1"/>
-      <color rgb="00FF07E6"/>
+      <color rgb="FFFF07E6"/>
       <sz val="12"/>
     </font>
   </fonts>
@@ -55,11 +55,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00B60C50"/>
+        <fgColor rgb="FFB60C50"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -67,18 +67,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <top style="dashed">
+        <color rgb="00FF0627"/>
+      </top>
+      <bottom style="double">
+        <color rgb="0006FF59"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,7 +471,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -483,7 +493,7 @@
         </is>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="19.5" customHeight="1" s="4">
       <c r="A2" t="inlineStr">
         <is>
           <t>John</t>
@@ -496,7 +506,7 @@
         <v>1760</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" ht="19.5" customHeight="1" s="4">
       <c r="A3" t="inlineStr">
         <is>
           <t>Bon</t>
@@ -509,7 +519,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" ht="22.5" customHeight="1" s="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
           <t>Kane</t>
@@ -522,20 +532,20 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="19.5" customHeight="1" s="4">
       <c r="A5" t="inlineStr">
         <is>
           <t>Tim</t>
         </is>
       </c>
-      <c r="B5" s="4" t="n">
+      <c r="B5" s="5" t="n">
         <v>1400</v>
       </c>
       <c r="C5" s="3" t="n">
         <v>2800</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" ht="19.5" customHeight="1" s="4">
       <c r="A6" t="inlineStr">
         <is>
           <t>Robin</t>
@@ -548,20 +558,20 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" ht="19.5" customHeight="1" s="4">
       <c r="A7" t="inlineStr">
         <is>
           <t>Michael</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" s="6" t="n">
         <v>780</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>1560</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" ht="19.5" customHeight="1" s="4">
       <c r="A8" t="inlineStr">
         <is>
           <t>Robert</t>

</xml_diff>

<commit_message>
execute excel formulas through python
</commit_message>
<xml_diff>
--- a/Openpyxl/Example.xlsx
+++ b/Openpyxl/Example.xlsx
@@ -1,119 +1,67 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT_Repositories\Openpyxl\Openpyxl\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2660F0B0-6DFA-4289-9402-4610D5AB1FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Balance" sheetId="1" r:id="rId1"/>
-    <sheet name="Score" sheetId="2" r:id="rId2"/>
+    <sheet name="Balance" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Score" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Balance</t>
-  </si>
-  <si>
-    <t>Double Balance</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Bon</t>
-  </si>
-  <si>
-    <t>Kane</t>
-  </si>
-  <si>
-    <t>Tim</t>
-  </si>
-  <si>
-    <t>Robin</t>
-  </si>
-  <si>
-    <t>Michael</t>
-  </si>
-  <si>
-    <t>Robert</t>
-  </si>
-  <si>
-    <t>Score</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Multiplier</t>
-  </si>
-  <si>
-    <t>Skill Level</t>
-  </si>
-  <si>
-    <t>Expert</t>
-  </si>
-  <si>
-    <t>2024-07-15</t>
-  </si>
-  <si>
-    <t>Beginner</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
-    <numFmt numFmtId="166" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Arial Black"/>
+      <color rgb="FF1807FF"/>
       <sz val="14"/>
-      <color rgb="FF1807FF"/>
-      <name val="Arial Black"/>
     </font>
     <font>
-      <b/>
-      <i/>
+      <name val="Arial Black"/>
+      <b val="1"/>
+      <i val="1"/>
+      <color rgb="FFFF07E6"/>
       <sz val="12"/>
-      <color rgb="FFFF07E6"/>
-      <name val="Arial Black"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <b val="1"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -147,49 +95,115 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="17">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0"/>
   </tableStyles>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -489,99 +503,204 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="13.77734375" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="13.109375" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="34.44140625" customWidth="1" min="5" max="5"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Balance</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Double Balance</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Interst Rare/Yr</t>
+        </is>
+      </c>
+      <c r="E1" s="16" t="inlineStr">
+        <is>
+          <t>Balance after a year</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="19.5" customHeight="1">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>880</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="3" t="n">
         <v>1760</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
+      <c r="D2" s="14" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E2" t="n">
+        <v>897.6</v>
+      </c>
+    </row>
+    <row r="3" ht="19.5" customHeight="1">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Bon</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>1200</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="3" t="n">
         <v>2400</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
+      <c r="D3" s="14" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="4" ht="22.5" customHeight="1">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Kane</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>1500</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="3" t="n">
         <v>3000</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4">
+      <c r="D4" s="14" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="5" ht="19.5" customHeight="1">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Tim</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="n">
         <v>1400</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="3" t="n">
         <v>2800</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
+      <c r="D5" s="14" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="6" ht="19.5" customHeight="1">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Robin</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>560</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="3" t="n">
         <v>1120</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="5">
+      <c r="D6" s="14" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="E6" t="n">
+        <v>599.2</v>
+      </c>
+    </row>
+    <row r="7" ht="19.5" customHeight="1">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+      <c r="B7" s="5" t="n">
         <v>780</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="3" t="n">
         <v>1560</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
+      <c r="D7" s="14" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="E7" t="n">
+        <v>811.2</v>
+      </c>
+    </row>
+    <row r="8" ht="19.5" customHeight="1">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Robert</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>920</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="3" t="n">
         <v>1840</v>
+      </c>
+      <c r="D8" s="14" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="E8" t="n">
+        <v>993.6</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>SUM</t>
+        </is>
+      </c>
+      <c r="B10">
+        <f>SUM(B2:B8)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Average</t>
+        </is>
+      </c>
+      <c r="B11">
+        <f>AVERAGE(B2:B8)</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -590,109 +709,143 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col width="9.109375" customWidth="1" style="6" min="1" max="2"/>
+    <col width="20.33203125" customWidth="1" min="3" max="3"/>
+    <col width="11.44140625" customWidth="1" min="4" max="4"/>
+    <col width="11.6640625" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="6">
+    <row r="1" customFormat="1" s="6">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="D1" s="6" t="inlineStr">
+        <is>
+          <t>Multiplier</t>
+        </is>
+      </c>
+      <c r="E1" s="15" t="inlineStr">
+        <is>
+          <t>Balance after a year</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="B2" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="13" t="n">
         <v>42209</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="8" t="n">
         <v>9</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="6">
+      <c r="E2" s="9" t="inlineStr">
+        <is>
+          <t>Expert</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="inlineStr">
+        <is>
+          <t>Bon</t>
+        </is>
+      </c>
+      <c r="B3" s="6" t="n">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="6">
+    <row r="4">
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t>Kane</t>
+        </is>
+      </c>
+      <c r="B4" s="6" t="n">
         <v>67</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="11">
+      <c r="C4" s="10" t="inlineStr">
+        <is>
+          <t>2024-07-15</t>
+        </is>
+      </c>
+      <c r="D4" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="6">
+      <c r="E4" s="12" t="inlineStr">
+        <is>
+          <t>Beginner</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t>Tim</t>
+        </is>
+      </c>
+      <c r="B5" s="6" t="n">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="6">
+    <row r="6">
+      <c r="A6" s="7" t="inlineStr">
+        <is>
+          <t>Robin</t>
+        </is>
+      </c>
+      <c r="B6" s="6" t="n">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="6">
+    <row r="7">
+      <c r="A7" s="7" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+      <c r="B7" s="6" t="n">
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="6">
+    <row r="8">
+      <c r="A8" s="7" t="inlineStr">
+        <is>
+          <t>Robert</t>
+        </is>
+      </c>
+      <c r="B8" s="6" t="n">
         <v>15</v>
       </c>
     </row>

</xml_diff>